<commit_message>
Correct c and d
</commit_message>
<xml_diff>
--- a/LR3/table_1_82.xlsx
+++ b/LR3/table_1_82.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E820B5-F71A-46B6-9C94-64DDECD3693E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6469856-699E-4427-A5B2-1E26D4A31409}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -548,7 +548,7 @@
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.42578125" defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -647,11 +647,11 @@
         <v>9</v>
       </c>
       <c r="C4" s="1">
-        <f>(C3-0.5)</f>
+        <f>C3-0.5</f>
         <v>69.5</v>
       </c>
       <c r="D4" s="1">
-        <f>A1*1.1</f>
+        <f>D3</f>
         <v>90.2</v>
       </c>
       <c r="E4" s="1">
@@ -692,11 +692,11 @@
         <v>10</v>
       </c>
       <c r="C5" s="1">
-        <f t="shared" ref="C5:C38" si="5">(C4-0.5)</f>
+        <f t="shared" ref="C5:C38" si="5">C4-0.5</f>
         <v>69</v>
       </c>
       <c r="D5" s="1">
-        <f>A1*1.1</f>
+        <f t="shared" ref="D5:D34" si="6">D4</f>
         <v>90.2</v>
       </c>
       <c r="E5" s="1">
@@ -704,11 +704,11 @@
         <v>6223.8</v>
       </c>
       <c r="F5" s="5">
-        <f t="shared" ref="F5:F38" si="6">F4</f>
+        <f t="shared" ref="F5:F38" si="7">F4</f>
         <v>44813</v>
       </c>
       <c r="G5" s="5">
-        <f t="shared" ref="G5:G38" si="7">G4+1</f>
+        <f t="shared" ref="G5:G38" si="8">G4+1</f>
         <v>44807</v>
       </c>
       <c r="H5" s="1">
@@ -716,7 +716,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="1">
-        <f t="shared" ref="I5:I38" si="8">I4</f>
+        <f t="shared" ref="I5:I38" si="9">I4</f>
         <v>10</v>
       </c>
       <c r="J5" s="1">
@@ -741,7 +741,7 @@
         <v>68.5</v>
       </c>
       <c r="D6" s="1">
-        <f>A1*1.1</f>
+        <f t="shared" si="6"/>
         <v>90.2</v>
       </c>
       <c r="E6" s="1">
@@ -749,11 +749,11 @@
         <v>6178.7</v>
       </c>
       <c r="F6" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G6" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44808</v>
       </c>
       <c r="H6" s="1">
@@ -761,7 +761,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="J6" s="1">
@@ -786,7 +786,7 @@
         <v>68</v>
       </c>
       <c r="D7" s="1">
-        <f>A1*1.1</f>
+        <f t="shared" si="6"/>
         <v>90.2</v>
       </c>
       <c r="E7" s="1">
@@ -794,11 +794,11 @@
         <v>6133.6</v>
       </c>
       <c r="F7" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G7" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44809</v>
       </c>
       <c r="H7" s="1">
@@ -806,7 +806,7 @@
         <v>0</v>
       </c>
       <c r="I7" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="J7" s="1">
@@ -831,7 +831,7 @@
         <v>67.5</v>
       </c>
       <c r="D8" s="1">
-        <f>A1*1.1</f>
+        <f t="shared" si="6"/>
         <v>90.2</v>
       </c>
       <c r="E8" s="1">
@@ -839,11 +839,11 @@
         <v>6088.5</v>
       </c>
       <c r="F8" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G8" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44810</v>
       </c>
       <c r="H8" s="1">
@@ -851,7 +851,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="J8" s="1">
@@ -876,7 +876,7 @@
         <v>67</v>
       </c>
       <c r="D9" s="1">
-        <f>A1*1.1</f>
+        <f t="shared" si="6"/>
         <v>90.2</v>
       </c>
       <c r="E9" s="1">
@@ -884,11 +884,11 @@
         <v>6043.4000000000005</v>
       </c>
       <c r="F9" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G9" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44811</v>
       </c>
       <c r="H9" s="1">
@@ -896,7 +896,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="J9" s="1">
@@ -921,7 +921,7 @@
         <v>66.5</v>
       </c>
       <c r="D10" s="1">
-        <f>A1*1.1</f>
+        <f t="shared" si="6"/>
         <v>90.2</v>
       </c>
       <c r="E10" s="1">
@@ -929,11 +929,11 @@
         <v>5998.3</v>
       </c>
       <c r="F10" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G10" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44812</v>
       </c>
       <c r="H10" s="1">
@@ -941,7 +941,7 @@
         <v>0</v>
       </c>
       <c r="I10" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="J10" s="1">
@@ -966,7 +966,7 @@
         <v>66</v>
       </c>
       <c r="D11" s="1">
-        <f>A1*1.1</f>
+        <f t="shared" si="6"/>
         <v>90.2</v>
       </c>
       <c r="E11" s="1">
@@ -974,11 +974,11 @@
         <v>5953.2</v>
       </c>
       <c r="F11" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G11" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44813</v>
       </c>
       <c r="H11" s="1">
@@ -986,7 +986,7 @@
         <v>0</v>
       </c>
       <c r="I11" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="J11" s="1">
@@ -1011,7 +1011,7 @@
         <v>65.5</v>
       </c>
       <c r="D12" s="1">
-        <f>A1*1.1</f>
+        <f t="shared" si="6"/>
         <v>90.2</v>
       </c>
       <c r="E12" s="1">
@@ -1019,11 +1019,11 @@
         <v>5908.1</v>
       </c>
       <c r="F12" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G12" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44814</v>
       </c>
       <c r="H12" s="1">
@@ -1031,7 +1031,7 @@
         <v>1</v>
       </c>
       <c r="I12" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="J12" s="1">
@@ -1056,7 +1056,7 @@
         <v>65</v>
       </c>
       <c r="D13" s="1">
-        <f>A1*1.1</f>
+        <f t="shared" si="6"/>
         <v>90.2</v>
       </c>
       <c r="E13" s="1">
@@ -1064,11 +1064,11 @@
         <v>5863</v>
       </c>
       <c r="F13" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G13" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44815</v>
       </c>
       <c r="H13" s="1">
@@ -1076,7 +1076,7 @@
         <v>2</v>
       </c>
       <c r="I13" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="J13" s="1">
@@ -1101,7 +1101,7 @@
         <v>64.5</v>
       </c>
       <c r="D14" s="1">
-        <f>A1*1.1</f>
+        <f t="shared" si="6"/>
         <v>90.2</v>
       </c>
       <c r="E14" s="1">
@@ -1109,11 +1109,11 @@
         <v>5817.9000000000005</v>
       </c>
       <c r="F14" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G14" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44816</v>
       </c>
       <c r="H14" s="1">
@@ -1121,7 +1121,7 @@
         <v>3</v>
       </c>
       <c r="I14" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="J14" s="1">
@@ -1146,7 +1146,7 @@
         <v>64</v>
       </c>
       <c r="D15" s="1">
-        <f>A1*1.1</f>
+        <f t="shared" si="6"/>
         <v>90.2</v>
       </c>
       <c r="E15" s="1">
@@ -1154,11 +1154,11 @@
         <v>5772.8</v>
       </c>
       <c r="F15" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G15" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44817</v>
       </c>
       <c r="H15" s="1">
@@ -1166,7 +1166,7 @@
         <v>4</v>
       </c>
       <c r="I15" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="J15" s="1">
@@ -1191,7 +1191,7 @@
         <v>63.5</v>
       </c>
       <c r="D16" s="1">
-        <f>A1*1.1</f>
+        <f t="shared" si="6"/>
         <v>90.2</v>
       </c>
       <c r="E16" s="1">
@@ -1199,11 +1199,11 @@
         <v>5727.7</v>
       </c>
       <c r="F16" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G16" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44818</v>
       </c>
       <c r="H16" s="1">
@@ -1211,7 +1211,7 @@
         <v>5</v>
       </c>
       <c r="I16" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="J16" s="1">
@@ -1236,7 +1236,7 @@
         <v>63</v>
       </c>
       <c r="D17" s="1">
-        <f>A1*1.1</f>
+        <f t="shared" si="6"/>
         <v>90.2</v>
       </c>
       <c r="E17" s="1">
@@ -1244,11 +1244,11 @@
         <v>5682.6</v>
       </c>
       <c r="F17" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G17" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44819</v>
       </c>
       <c r="H17" s="1">
@@ -1256,7 +1256,7 @@
         <v>6</v>
       </c>
       <c r="I17" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="J17" s="1">
@@ -1281,7 +1281,7 @@
         <v>62.5</v>
       </c>
       <c r="D18" s="1">
-        <f>A1*1.1</f>
+        <f t="shared" si="6"/>
         <v>90.2</v>
       </c>
       <c r="E18" s="1">
@@ -1289,11 +1289,11 @@
         <v>5637.5</v>
       </c>
       <c r="F18" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G18" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44820</v>
       </c>
       <c r="H18" s="1">
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="I18" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="J18" s="1">
@@ -1326,7 +1326,7 @@
         <v>62</v>
       </c>
       <c r="D19" s="1">
-        <f>A1*1.1</f>
+        <f t="shared" si="6"/>
         <v>90.2</v>
       </c>
       <c r="E19" s="1">
@@ -1334,11 +1334,11 @@
         <v>5592.4000000000005</v>
       </c>
       <c r="F19" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G19" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44821</v>
       </c>
       <c r="H19" s="1">
@@ -1346,7 +1346,7 @@
         <v>8</v>
       </c>
       <c r="I19" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="J19" s="1">
@@ -1371,7 +1371,7 @@
         <v>61.5</v>
       </c>
       <c r="D20" s="1">
-        <f>A1*1.1</f>
+        <f t="shared" si="6"/>
         <v>90.2</v>
       </c>
       <c r="E20" s="1">
@@ -1379,11 +1379,11 @@
         <v>5547.3</v>
       </c>
       <c r="F20" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G20" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44822</v>
       </c>
       <c r="H20" s="1">
@@ -1391,7 +1391,7 @@
         <v>9</v>
       </c>
       <c r="I20" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="J20" s="1">
@@ -1416,7 +1416,7 @@
         <v>61</v>
       </c>
       <c r="D21" s="1">
-        <f>A1*1.1</f>
+        <f t="shared" si="6"/>
         <v>90.2</v>
       </c>
       <c r="E21" s="1">
@@ -1424,11 +1424,11 @@
         <v>5502.2</v>
       </c>
       <c r="F21" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G21" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44823</v>
       </c>
       <c r="H21" s="1">
@@ -1436,7 +1436,7 @@
         <v>10</v>
       </c>
       <c r="I21" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="J21" s="1">
@@ -1461,7 +1461,7 @@
         <v>60.5</v>
       </c>
       <c r="D22" s="1">
-        <f>A1*1.1</f>
+        <f t="shared" si="6"/>
         <v>90.2</v>
       </c>
       <c r="E22" s="1">
@@ -1469,11 +1469,11 @@
         <v>5457.1</v>
       </c>
       <c r="F22" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G22" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44824</v>
       </c>
       <c r="H22" s="1">
@@ -1481,7 +1481,7 @@
         <v>11</v>
       </c>
       <c r="I22" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="J22" s="1">
@@ -1506,7 +1506,7 @@
         <v>60</v>
       </c>
       <c r="D23" s="1">
-        <f>A1*1.1</f>
+        <f t="shared" si="6"/>
         <v>90.2</v>
       </c>
       <c r="E23" s="1">
@@ -1514,11 +1514,11 @@
         <v>5412</v>
       </c>
       <c r="F23" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G23" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44825</v>
       </c>
       <c r="H23" s="1">
@@ -1526,7 +1526,7 @@
         <v>12</v>
       </c>
       <c r="I23" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="J23" s="1">
@@ -1551,7 +1551,7 @@
         <v>59.5</v>
       </c>
       <c r="D24" s="1">
-        <f>A1*1.1</f>
+        <f t="shared" si="6"/>
         <v>90.2</v>
       </c>
       <c r="E24" s="1">
@@ -1559,11 +1559,11 @@
         <v>5366.9000000000005</v>
       </c>
       <c r="F24" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G24" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44826</v>
       </c>
       <c r="H24" s="1">
@@ -1571,7 +1571,7 @@
         <v>13</v>
       </c>
       <c r="I24" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="J24" s="1">
@@ -1596,7 +1596,7 @@
         <v>59</v>
       </c>
       <c r="D25" s="1">
-        <f>A1*1.1</f>
+        <f t="shared" si="6"/>
         <v>90.2</v>
       </c>
       <c r="E25" s="1">
@@ -1604,11 +1604,11 @@
         <v>5321.8</v>
       </c>
       <c r="F25" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G25" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44827</v>
       </c>
       <c r="H25" s="1">
@@ -1616,7 +1616,7 @@
         <v>14</v>
       </c>
       <c r="I25" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="J25" s="1">
@@ -1641,7 +1641,7 @@
         <v>58.5</v>
       </c>
       <c r="D26" s="1">
-        <f>A1*1.1</f>
+        <f t="shared" si="6"/>
         <v>90.2</v>
       </c>
       <c r="E26" s="1">
@@ -1649,11 +1649,11 @@
         <v>5276.7</v>
       </c>
       <c r="F26" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G26" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44828</v>
       </c>
       <c r="H26" s="1">
@@ -1661,7 +1661,7 @@
         <v>15</v>
       </c>
       <c r="I26" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="J26" s="1">
@@ -1686,7 +1686,7 @@
         <v>58</v>
       </c>
       <c r="D27" s="1">
-        <f>A1*1.1</f>
+        <f t="shared" si="6"/>
         <v>90.2</v>
       </c>
       <c r="E27" s="1">
@@ -1694,11 +1694,11 @@
         <v>5231.6000000000004</v>
       </c>
       <c r="F27" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G27" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44829</v>
       </c>
       <c r="H27" s="1">
@@ -1706,7 +1706,7 @@
         <v>16</v>
       </c>
       <c r="I27" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="J27" s="1">
@@ -1731,7 +1731,7 @@
         <v>57.5</v>
       </c>
       <c r="D28" s="1">
-        <f>A1*1.1</f>
+        <f t="shared" si="6"/>
         <v>90.2</v>
       </c>
       <c r="E28" s="1">
@@ -1739,11 +1739,11 @@
         <v>5186.5</v>
       </c>
       <c r="F28" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G28" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44830</v>
       </c>
       <c r="H28" s="1">
@@ -1751,7 +1751,7 @@
         <v>17</v>
       </c>
       <c r="I28" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="J28" s="1">
@@ -1776,7 +1776,7 @@
         <v>57</v>
       </c>
       <c r="D29" s="1">
-        <f>A1*1.1</f>
+        <f t="shared" si="6"/>
         <v>90.2</v>
       </c>
       <c r="E29" s="1">
@@ -1784,11 +1784,11 @@
         <v>5141.4000000000005</v>
       </c>
       <c r="F29" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G29" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44831</v>
       </c>
       <c r="H29" s="1">
@@ -1796,7 +1796,7 @@
         <v>18</v>
       </c>
       <c r="I29" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="J29" s="1">
@@ -1821,7 +1821,7 @@
         <v>56.5</v>
       </c>
       <c r="D30" s="1">
-        <f>A1*1.1</f>
+        <f t="shared" si="6"/>
         <v>90.2</v>
       </c>
       <c r="E30" s="1">
@@ -1829,11 +1829,11 @@
         <v>5096.3</v>
       </c>
       <c r="F30" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G30" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44832</v>
       </c>
       <c r="H30" s="1">
@@ -1841,7 +1841,7 @@
         <v>19</v>
       </c>
       <c r="I30" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="J30" s="1">
@@ -1866,7 +1866,7 @@
         <v>56</v>
       </c>
       <c r="D31" s="1">
-        <f>A1*1.1</f>
+        <f t="shared" si="6"/>
         <v>90.2</v>
       </c>
       <c r="E31" s="1">
@@ -1874,11 +1874,11 @@
         <v>5051.2</v>
       </c>
       <c r="F31" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G31" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44833</v>
       </c>
       <c r="H31" s="1">
@@ -1886,7 +1886,7 @@
         <v>20</v>
       </c>
       <c r="I31" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="J31" s="1">
@@ -1911,7 +1911,7 @@
         <v>55.5</v>
       </c>
       <c r="D32" s="1">
-        <f>A1*1.1</f>
+        <f t="shared" si="6"/>
         <v>90.2</v>
       </c>
       <c r="E32" s="1">
@@ -1919,11 +1919,11 @@
         <v>5006.1000000000004</v>
       </c>
       <c r="F32" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G32" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44834</v>
       </c>
       <c r="H32" s="1">
@@ -1931,7 +1931,7 @@
         <v>21</v>
       </c>
       <c r="I32" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="J32" s="1">
@@ -1956,7 +1956,7 @@
         <v>55</v>
       </c>
       <c r="D33" s="1">
-        <f>A1*1.1</f>
+        <f t="shared" si="6"/>
         <v>90.2</v>
       </c>
       <c r="E33" s="1">
@@ -1964,11 +1964,11 @@
         <v>4961</v>
       </c>
       <c r="F33" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G33" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44835</v>
       </c>
       <c r="H33" s="1">
@@ -1976,7 +1976,7 @@
         <v>22</v>
       </c>
       <c r="I33" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="J33" s="1">
@@ -2001,7 +2001,7 @@
         <v>54.5</v>
       </c>
       <c r="D34" s="1">
-        <f>A1*1.1</f>
+        <f t="shared" si="6"/>
         <v>90.2</v>
       </c>
       <c r="E34" s="1">
@@ -2009,11 +2009,11 @@
         <v>4915.9000000000005</v>
       </c>
       <c r="F34" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G34" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44836</v>
       </c>
       <c r="H34" s="1">
@@ -2021,7 +2021,7 @@
         <v>23</v>
       </c>
       <c r="I34" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="J34" s="1">
@@ -2054,11 +2054,11 @@
         <v>2435.4</v>
       </c>
       <c r="F35" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G35" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44837</v>
       </c>
       <c r="H35" s="1">
@@ -2066,7 +2066,7 @@
         <v>24</v>
       </c>
       <c r="I35" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="J35" s="1">
@@ -2091,7 +2091,7 @@
         <v>53.5</v>
       </c>
       <c r="D36" s="1">
-        <f>A1*1.1/2</f>
+        <f>D35</f>
         <v>45.1</v>
       </c>
       <c r="E36" s="1">
@@ -2099,11 +2099,11 @@
         <v>2412.85</v>
       </c>
       <c r="F36" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G36" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44838</v>
       </c>
       <c r="H36" s="1">
@@ -2111,7 +2111,7 @@
         <v>25</v>
       </c>
       <c r="I36" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="J36" s="1">
@@ -2136,7 +2136,7 @@
         <v>53</v>
       </c>
       <c r="D37" s="1">
-        <f>A1*1.1/2</f>
+        <f t="shared" ref="D37:D38" si="10">D36</f>
         <v>45.1</v>
       </c>
       <c r="E37" s="1">
@@ -2144,11 +2144,11 @@
         <v>2390.3000000000002</v>
       </c>
       <c r="F37" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G37" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44839</v>
       </c>
       <c r="H37" s="1">
@@ -2156,7 +2156,7 @@
         <v>26</v>
       </c>
       <c r="I37" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="J37" s="1">
@@ -2181,7 +2181,7 @@
         <v>52.5</v>
       </c>
       <c r="D38" s="1">
-        <f>A1*1.1/2</f>
+        <f t="shared" si="10"/>
         <v>45.1</v>
       </c>
       <c r="E38" s="1">
@@ -2189,11 +2189,11 @@
         <v>2367.75</v>
       </c>
       <c r="F38" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44813</v>
       </c>
       <c r="G38" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44840</v>
       </c>
       <c r="H38" s="1">
@@ -2201,7 +2201,7 @@
         <v>27</v>
       </c>
       <c r="I38" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="J38" s="1">

</xml_diff>